<commit_message>
add column calculation type and blacklist filter
</commit_message>
<xml_diff>
--- a/app/assets/excel/template_mass_upload_discount.xlsx
+++ b/app/assets/excel/template_mass_upload_discount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BE-POS\app\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724F65C6-9FD4-44EB-BA4D-8B950C855BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E94F92F-34D6-4BE5-A306-727474D9A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="84" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{0A217623-5B23-4BCD-B0A8-7C78302A134B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0A217623-5B23-4BCD-B0A8-7C78302A134B}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Kode Supplier</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>tidak diisi dianggap semua kode item</t>
-  </si>
-  <si>
-    <t>diskon per sersentase tanpa symbol persen(%)</t>
   </si>
   <si>
     <t>Level</t>
@@ -105,13 +102,32 @@
   <si>
     <t>format 
 dd/mm/yyyy  HH:MM</t>
+  </si>
+  <si>
+    <t>Tipe Kalkulasi</t>
+  </si>
+  <si>
+    <t>percentage untuk diskon dengan persentase, nominal untuk diskon dengan fixed value</t>
+  </si>
+  <si>
+    <t>Value diskon sesuai tipe kalkulasi</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>nominal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +145,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -173,10 +196,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -188,8 +212,16 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B061825D-5C2F-48CA-8BAB-260ECE19E42B}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +545,7 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="13" customWidth="1"/>
     <col min="5" max="5" width="22.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.21875" customWidth="1"/>
     <col min="7" max="7" width="17.21875" customWidth="1"/>
@@ -521,9 +553,10 @@
     <col min="9" max="9" width="20.21875" customWidth="1"/>
     <col min="10" max="10" width="21.77734375" style="6" customWidth="1"/>
     <col min="11" max="11" width="21.44140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,32 +566,35 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -568,102 +604,105 @@
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
@@ -671,16 +710,21 @@
       <c r="I9" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{A490029A-A4BB-455D-9CEE-5F139E408DCF}">
+      <formula1>"percentage,nominal"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915F154E-7372-47F4-9952-566B5E17D842}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,16 +732,16 @@
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="21.77734375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" style="6" customWidth="1"/>
+    <col min="4" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,28 +755,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="78" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -746,128 +793,143 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
+      <c r="D3" s="10"/>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="9">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="8">
+      <c r="J3" s="4"/>
+      <c r="K3" s="8">
         <v>45323</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
+      <c r="D4" s="10"/>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="9">
         <v>2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>8</v>
       </c>
-      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="8">
+      <c r="J4" s="4"/>
+      <c r="K4" s="8">
         <v>45323</v>
       </c>
-      <c r="K4" s="8">
+      <c r="L4" s="8">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
+      <c r="D5" s="10"/>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="9">
         <v>3</v>
       </c>
-      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="8">
+      <c r="J5" s="4"/>
+      <c r="K5" s="8">
         <v>45323</v>
       </c>
-      <c r="K5" s="8">
+      <c r="L5" s="8">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <v>230912345</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="9">
         <v>4</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>9</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>10</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>11</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>45323</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="8">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -875,24 +937,27 @@
         <v>8</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3">
+      <c r="D7" s="10"/>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
-        <v>5</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="9">
+        <v>5000</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="8">
+      <c r="J7" s="4"/>
+      <c r="K7" s="8">
         <v>45323</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -900,24 +965,27 @@
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="D8" s="10"/>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="4">
-        <v>6</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="9">
+        <v>60000</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="8">
+      <c r="J8" s="4"/>
+      <c r="K8" s="8">
         <v>45292</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="8">
         <v>45657.999305555553</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -925,34 +993,42 @@
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3">
+      <c r="D9" s="10"/>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3">
         <v>3</v>
       </c>
-      <c r="F9" s="4">
-        <v>7</v>
-      </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="9">
+        <v>700</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="8">
+      <c r="J9" s="4"/>
+      <c r="K9" s="8">
         <v>45292</v>
       </c>
-      <c r="K9" s="8">
+      <c r="L9" s="8">
         <v>45657.999305555553</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F12" s="7"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G12" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zO6nmUs3L5QA7FVvfXt/W40pgWLcQfQvpzMqwjgyAtXUsVTxh2Ayf5IIhLU4PFClIY+3yUJWq22fGc27fw0Mvg==" saltValue="/Bu00JKgeiYXCP9GIDqcLA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ycfkmUzppvW36ZL1fQOpEqNyxn+fjq7rprcxBseOZAXByKHEihB0FMVKqLXPPZaLhKTxMvhvnNVeKckp4lm3+Q==" saltValue="WKQPBRIHBo2oJaLiljI6KQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{66E46FB1-915A-4C23-B6D1-F33262D52E17}">
+      <formula1>"percentage,nominal"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix error read excel due example tab
</commit_message>
<xml_diff>
--- a/app/assets/excel/template_mass_upload_discount.xlsx
+++ b/app/assets/excel/template_mass_upload_discount.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BE-POS\app\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E94F92F-34D6-4BE5-A306-727474D9A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE69FCD-E7AA-42A0-8515-98F24D2DA0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0A217623-5B23-4BCD-B0A8-7C78302A134B}"/>
+    <workbookView xWindow="1440" yWindow="1224" windowWidth="21600" windowHeight="12456" activeTab="1" xr2:uid="{0A217623-5B23-4BCD-B0A8-7C78302A134B}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
-    <sheet name="Contoh" sheetId="1" r:id="rId2"/>
+    <sheet name="contoh" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -123,10 +123,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,6 +147,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -196,11 +193,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -210,18 +206,18 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B061825D-5C2F-48CA-8BAB-260ECE19E42B}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -545,7 +541,7 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="10" customWidth="1"/>
     <col min="5" max="5" width="22.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.21875" customWidth="1"/>
     <col min="7" max="7" width="17.21875" customWidth="1"/>
@@ -566,7 +562,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -604,7 +600,7 @@
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -636,7 +632,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
@@ -647,7 +643,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="10"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
@@ -658,7 +654,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="10"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
@@ -669,7 +665,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -680,7 +676,7 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
@@ -691,7 +687,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -702,7 +698,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="10"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
@@ -720,315 +716,265 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915F154E-7372-47F4-9952-566B5E17D842}">
-  <dimension ref="A1:L12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D860E9E9-C007-44C0-9157-4F63EB3DE4A6}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="7" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="8">
+      <c r="K3" s="6">
         <v>45323</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>8</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="8">
+      <c r="K4" s="6">
         <v>45323</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="6">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="8">
+      <c r="K5" s="6">
         <v>45323</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="10">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D6">
         <v>230912345</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>9</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>10</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>11</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="6">
         <v>45323</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7">
         <v>5000</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="8">
+      <c r="K7" s="6">
         <v>45323</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="6">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8">
         <v>60000</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="8">
+      <c r="K8" s="6">
         <v>45292</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <v>45657.999305555553</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9">
         <v>700</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="8">
+      <c r="K9" s="6">
         <v>45292</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="6">
         <v>45657.999305555553</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G12" s="7"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ycfkmUzppvW36ZL1fQOpEqNyxn+fjq7rprcxBseOZAXByKHEihB0FMVKqLXPPZaLhKTxMvhvnNVeKckp4lm3+Q==" saltValue="WKQPBRIHBo2oJaLiljI6KQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{66E46FB1-915A-4C23-B6D1-F33262D52E17}">
-      <formula1>"percentage,nominal"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <sheetProtection algorithmName="SHA-512" hashValue="gqqCImjqarJYxNIxDOaXUAAzjJWGFZKO7l2LlDZGfichYpN1FIRYunrzztjNzOJ5U96P+NGB1hgVa+4ON79RAg==" saltValue="K8HXHoeJnrSakwOkNPJxOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bug cache should remove when item updated
</commit_message>
<xml_diff>
--- a/app/assets/excel/template_mass_upload_discount.xlsx
+++ b/app/assets/excel/template_mass_upload_discount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BE-POS\app\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE69FCD-E7AA-42A0-8515-98F24D2DA0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA5862A-C808-4C9C-93F6-A7908CD2F21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1224" windowWidth="21600" windowHeight="12456" activeTab="1" xr2:uid="{0A217623-5B23-4BCD-B0A8-7C78302A134B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0A217623-5B23-4BCD-B0A8-7C78302A134B}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>Kode Supplier</t>
   </si>
@@ -100,23 +100,35 @@
     <t>Tanggal Akhir</t>
   </si>
   <si>
-    <t>format 
+    <t>Tipe Kalkulasi</t>
+  </si>
+  <si>
+    <t>percentage untuk diskon dengan persentase, nominal untuk diskon dengan fixed value</t>
+  </si>
+  <si>
+    <t>Value diskon sesuai tipe kalkulasi</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>Kode</t>
+  </si>
+  <si>
+    <t>kode diskon. Jika tidak diisi akan digenerate oleh system</t>
+  </si>
+  <si>
+    <t>promosi lebaran</t>
+  </si>
+  <si>
+    <t>wajib diisi. format 
 dd/mm/yyyy  HH:MM</t>
   </si>
   <si>
-    <t>Tipe Kalkulasi</t>
-  </si>
-  <si>
-    <t>percentage untuk diskon dengan persentase, nominal untuk diskon dengan fixed value</t>
-  </si>
-  <si>
-    <t>Value diskon sesuai tipe kalkulasi</t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
-    <t>nominal</t>
+    <t>promosi natal</t>
   </si>
 </sst>
 </file>
@@ -530,184 +542,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B061825D-5C2F-48CA-8BAB-260ECE19E42B}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" customWidth="1"/>
-    <col min="10" max="10" width="21.77734375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="78" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="78" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{A490029A-A4BB-455D-9CEE-5F139E408DCF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{A490029A-A4BB-455D-9CEE-5F139E408DCF}">
       <formula1>"percentage,nominal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -717,264 +736,357 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D860E9E9-C007-44C0-9157-4F63EB3DE4A6}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" customWidth="1"/>
-    <col min="7" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="8" max="11" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="I2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="K3" s="6">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6">
         <v>45323</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>45351.999305555553</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45323</v>
+      </c>
+      <c r="M4" s="6">
+        <v>45351.999305555553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45323</v>
+      </c>
+      <c r="M5" s="6">
+        <v>45351.999305555553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>230912345</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6" s="6">
+        <v>45323</v>
+      </c>
+      <c r="M6" s="6">
+        <v>45351.999305555553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F4">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="H7">
+        <v>5000</v>
+      </c>
+      <c r="L7" s="6">
+        <v>45323</v>
+      </c>
+      <c r="M7" s="6">
+        <v>45351.999305555553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>8</v>
-      </c>
-      <c r="K4" s="6">
-        <v>45323</v>
-      </c>
-      <c r="L4" s="6">
-        <v>45351.999305555553</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="H8">
+        <v>60000</v>
+      </c>
+      <c r="L8" s="6">
+        <v>45292</v>
+      </c>
+      <c r="M8" s="6">
+        <v>45657.999305555553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
         <v>28</v>
       </c>
-      <c r="F5">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>700</v>
+      </c>
+      <c r="L9" s="6">
+        <v>45292</v>
+      </c>
+      <c r="M9" s="6">
+        <v>45657.999305555553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>23010010</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="K5" s="6">
-        <v>45323</v>
-      </c>
-      <c r="L5" s="6">
-        <v>45351.999305555553</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>230912345</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
+      <c r="H10">
         <v>10</v>
       </c>
-      <c r="J6">
-        <v>11</v>
-      </c>
-      <c r="K6" s="6">
-        <v>45323</v>
-      </c>
-      <c r="L6" s="6">
-        <v>45351.999305555553</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7">
+      <c r="L10" s="6">
+        <v>45292</v>
+      </c>
+      <c r="M10" s="6">
+        <v>45657.999305555553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>23010012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>23110258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <v>23127323</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>5000</v>
-      </c>
-      <c r="K7" s="6">
-        <v>45323</v>
-      </c>
-      <c r="L7" s="6">
-        <v>45351.999305555553</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>60000</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="H13">
+        <v>15</v>
+      </c>
+      <c r="L13" s="6">
         <v>45292</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M13" s="6">
         <v>45657.999305555553</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>700</v>
-      </c>
-      <c r="K9" s="6">
-        <v>45292</v>
-      </c>
-      <c r="L9" s="6">
-        <v>45657.999305555553</v>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>23127325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>23127327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16">
+        <v>23127328</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gqqCImjqarJYxNIxDOaXUAAzjJWGFZKO7l2LlDZGfichYpN1FIRYunrzztjNzOJ5U96P+NGB1hgVa+4ON79RAg==" saltValue="K8HXHoeJnrSakwOkNPJxOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="t4Sr9JpQSfBhUoMHbEnXTjw2xAp+1Uko7JN+uVQXJf7bXGNU4qtuWSTjt1vZpWuvbCpnHr8gdCCJy6dPrISSeQ==" saltValue="o7F4k4XL1Sg+3ehOn0s3Bw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>